<commit_message>
Updated code for nowcasting_1
</commit_message>
<xml_diff>
--- a/gdp_revisions_analysis_jefas/input/data/Nowcasting_Performance_EVAL_split_2013.xlsx
+++ b/gdp_revisions_analysis_jefas/input/data/Nowcasting_Performance_EVAL_split_2013.xlsx
@@ -13,18 +13,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" count="4" uniqueCount="4">
   <si>
     <t>Horizon</t>
   </si>
   <si>
-    <t>MAE (Bench=100)</t>
-  </si>
-  <si>
     <t>RMSE (Bench=100)</t>
-  </si>
-  <si>
-    <t>MAPE (Bench=100)</t>
   </si>
   <si>
     <t>DM stat</t>
@@ -76,7 +70,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F12"/>
+  <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -95,31 +89,19 @@
       <c r="D1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" t="s">
-        <v>5</v>
-      </c>
     </row>
     <row r="2">
       <c r="A2" s="1">
         <v>1</v>
       </c>
       <c r="B2" s="1">
-        <v>82.175384521484375</v>
+        <v>148.39120483398438</v>
       </c>
       <c r="C2" s="1">
-        <v>65.061141967773438</v>
+        <v>4.9638833999633789</v>
       </c>
       <c r="D2" s="1">
-        <v>95.055953979492188</v>
-      </c>
-      <c r="E2" s="1">
-        <v>-2.7785227298736572</v>
-      </c>
-      <c r="F2" s="1">
-        <v>81.53765869140625</v>
+        <v>25.895881652832031</v>
       </c>
     </row>
     <row r="3">
@@ -127,19 +109,13 @@
         <v>2</v>
       </c>
       <c r="B3" s="1">
-        <v>77.066902160644531</v>
+        <v>143.82656860351562</v>
       </c>
       <c r="C3" s="1">
-        <v>61.021018981933594</v>
+        <v>4.0256404876708984</v>
       </c>
       <c r="D3" s="1">
-        <v>84.022918701171875</v>
-      </c>
-      <c r="E3" s="1">
-        <v>-3.3394458293914795</v>
-      </c>
-      <c r="F3" s="1">
-        <v>46.848194122314453</v>
+        <v>14.725439071655273</v>
       </c>
     </row>
     <row r="4">
@@ -147,19 +123,13 @@
         <v>3</v>
       </c>
       <c r="B4" s="1">
-        <v>73.190773010253906</v>
+        <v>127.17751312255859</v>
       </c>
       <c r="C4" s="1">
-        <v>58.289695739746094</v>
+        <v>2.2624156475067139</v>
       </c>
       <c r="D4" s="1">
-        <v>63.010562896728516</v>
-      </c>
-      <c r="E4" s="1">
-        <v>-3.5438356399536133</v>
-      </c>
-      <c r="F4" s="1">
-        <v>25.064416885375977</v>
+        <v>8.1826372146606445</v>
       </c>
     </row>
     <row r="5">
@@ -167,19 +137,13 @@
         <v>4</v>
       </c>
       <c r="B5" s="1">
-        <v>50.509803771972656</v>
+        <v>87.526031494140625</v>
       </c>
       <c r="C5" s="1">
-        <v>38.744205474853516</v>
+        <v>-0.93605679273605347</v>
       </c>
       <c r="D5" s="1">
-        <v>40.466133117675781</v>
-      </c>
-      <c r="E5" s="1">
-        <v>-4.1170234680175781</v>
-      </c>
-      <c r="F5" s="1">
-        <v>59.511241912841797</v>
+        <v>14.976428985595703</v>
       </c>
     </row>
     <row r="6">
@@ -187,19 +151,13 @@
         <v>5</v>
       </c>
       <c r="B6" s="1">
-        <v>36.241809844970703</v>
+        <v>47.085796356201172</v>
       </c>
       <c r="C6" s="1">
-        <v>28.718009948730469</v>
+        <v>-3.5409884452819824</v>
       </c>
       <c r="D6" s="1">
-        <v>31.176292419433594</v>
-      </c>
-      <c r="E6" s="1">
-        <v>-4.2824134826660156</v>
-      </c>
-      <c r="F6" s="1">
-        <v>52.607810974121094</v>
+        <v>24.640964508056641</v>
       </c>
     </row>
     <row r="7">
@@ -207,19 +165,13 @@
         <v>6</v>
       </c>
       <c r="B7" s="1">
-        <v>44.5875244140625</v>
+        <v>68.021408081054688</v>
       </c>
       <c r="C7" s="1">
-        <v>39.516185760498047</v>
+        <v>-2.1883008480072021</v>
       </c>
       <c r="D7" s="1">
-        <v>39.446125030517578</v>
-      </c>
-      <c r="E7" s="1">
-        <v>-4.2866425514221191</v>
-      </c>
-      <c r="F7" s="1">
-        <v>16.809812545776367</v>
+        <v>7.0427446365356445</v>
       </c>
     </row>
     <row r="8">
@@ -227,19 +179,13 @@
         <v>7</v>
       </c>
       <c r="B8" s="1">
-        <v>36.747631072998047</v>
+        <v>44.554885864257812</v>
       </c>
       <c r="C8" s="1">
-        <v>28.855743408203125</v>
+        <v>-3.2349586486816406</v>
       </c>
       <c r="D8" s="1">
-        <v>38.189437866210938</v>
-      </c>
-      <c r="E8" s="1">
-        <v>-3.4541804790496826</v>
-      </c>
-      <c r="F8" s="1">
-        <v>21.628211975097656</v>
+        <v>13.491148948669434</v>
       </c>
     </row>
     <row r="9">
@@ -247,19 +193,13 @@
         <v>8</v>
       </c>
       <c r="B9" s="1">
-        <v>31.101720809936523</v>
+        <v>20.84794807434082</v>
       </c>
       <c r="C9" s="1">
-        <v>21.499444961547852</v>
+        <v>-3.1974742412567139</v>
       </c>
       <c r="D9" s="1">
-        <v>30.954399108886719</v>
-      </c>
-      <c r="E9" s="1">
-        <v>-3.1914265155792236</v>
-      </c>
-      <c r="F9" s="1">
-        <v>43.323638916015625</v>
+        <v>44.267559051513672</v>
       </c>
     </row>
     <row r="10">
@@ -267,19 +207,13 @@
         <v>9</v>
       </c>
       <c r="B10" s="1">
-        <v>86.664352416992188</v>
+        <v>55.5565185546875</v>
       </c>
       <c r="C10" s="1">
-        <v>48.051910400390625</v>
+        <v>-3.1716289520263672</v>
       </c>
       <c r="D10" s="1">
-        <v>140.38107299804688</v>
-      </c>
-      <c r="E10" s="1">
-        <v>-3.5955665111541748</v>
-      </c>
-      <c r="F10" s="1">
-        <v>44.746917724609375</v>
+        <v>34.436431884765625</v>
       </c>
     </row>
     <row r="11">
@@ -287,19 +221,13 @@
         <v>10</v>
       </c>
       <c r="B11" s="1">
-        <v>137.78962707519531</v>
+        <v>97.905319213867188</v>
       </c>
       <c r="C11" s="1">
-        <v>62.502063751220703</v>
+        <v>-0.14818011224269867</v>
       </c>
       <c r="D11" s="1">
-        <v>218.33613586425781</v>
-      </c>
-      <c r="E11" s="1">
-        <v>-2.4863367080688477</v>
-      </c>
-      <c r="F11" s="1">
-        <v>55.117694854736328</v>
+        <v>35.524921417236328</v>
       </c>
     </row>
     <row r="12">
@@ -307,19 +235,13 @@
         <v>11</v>
       </c>
       <c r="B12" s="1">
-        <v>36.068157196044922</v>
+        <v>53.46929931640625</v>
       </c>
       <c r="C12" s="1">
-        <v>11.378140449523926</v>
+        <v>-1.9795914888381958</v>
       </c>
       <c r="D12" s="1">
-        <v>54.614810943603516</v>
-      </c>
-      <c r="E12" s="1">
-        <v>-2.7501277923583984</v>
-      </c>
-      <c r="F12" s="1">
-        <v>308.81793212890625</v>
+        <v>44.606975555419922</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated real time exercise with h-specific delta
</commit_message>
<xml_diff>
--- a/gdp_revisions_analysis_jefas/input/data/Nowcasting_Performance_EVAL_split_2013.xlsx
+++ b/gdp_revisions_analysis_jefas/input/data/Nowcasting_Performance_EVAL_split_2013.xlsx
@@ -95,13 +95,13 @@
         <v>1</v>
       </c>
       <c r="B2" s="1">
-        <v>110.68733978271484</v>
+        <v>89.933845520019531</v>
       </c>
       <c r="C2" s="1">
-        <v>0.73834848403930664</v>
+        <v>-0.82123315334320068</v>
       </c>
       <c r="D2" s="1">
-        <v>0.58858436346054077</v>
+        <v>0.24532508850097656</v>
       </c>
     </row>
     <row r="3">
@@ -109,13 +109,13 @@
         <v>2</v>
       </c>
       <c r="B3" s="1">
-        <v>107.13040924072266</v>
+        <v>87.274131774902344</v>
       </c>
       <c r="C3" s="1">
-        <v>0.48421236872673035</v>
+        <v>-1.0597113370895386</v>
       </c>
       <c r="D3" s="1">
-        <v>1.2130931615829468</v>
+        <v>0.91008186340332031</v>
       </c>
     </row>
     <row r="4">
@@ -123,13 +123,13 @@
         <v>3</v>
       </c>
       <c r="B4" s="1">
-        <v>104.14569091796875</v>
+        <v>91.155021667480469</v>
       </c>
       <c r="C4" s="1">
-        <v>0.30985361337661743</v>
+        <v>-0.89096373319625854</v>
       </c>
       <c r="D4" s="1">
-        <v>2.6056814193725586</v>
+        <v>2.4081621170043945</v>
       </c>
     </row>
     <row r="5">
@@ -137,13 +137,13 @@
         <v>4</v>
       </c>
       <c r="B5" s="1">
-        <v>101.14502716064453</v>
+        <v>92.403213500976562</v>
       </c>
       <c r="C5" s="1">
-        <v>0.11792938411235809</v>
+        <v>-1.1595971584320068</v>
       </c>
       <c r="D5" s="1">
-        <v>1.2559480667114258</v>
+        <v>1.2837705612182617</v>
       </c>
     </row>
     <row r="6">
@@ -151,13 +151,13 @@
         <v>5</v>
       </c>
       <c r="B6" s="1">
-        <v>101.46086120605469</v>
+        <v>100.34432220458984</v>
       </c>
       <c r="C6" s="1">
-        <v>0.30565011501312256</v>
+        <v>0.10446625947952271</v>
       </c>
       <c r="D6" s="1">
-        <v>-0.50412899255752563</v>
+        <v>-0.71237343549728394</v>
       </c>
     </row>
     <row r="7">
@@ -165,13 +165,13 @@
         <v>6</v>
       </c>
       <c r="B7" s="1">
-        <v>101.52155303955078</v>
+        <v>100.99150085449219</v>
       </c>
       <c r="C7" s="1">
-        <v>0.21311436593532562</v>
+        <v>0.17972996830940247</v>
       </c>
       <c r="D7" s="1">
-        <v>2.413261890411377</v>
+        <v>1.9403207302093506</v>
       </c>
     </row>
     <row r="8">
@@ -179,13 +179,13 @@
         <v>7</v>
       </c>
       <c r="B8" s="1">
-        <v>99.152023315429688</v>
+        <v>95.411331176757812</v>
       </c>
       <c r="C8" s="1">
-        <v>-0.13095328211784363</v>
+        <v>-0.65167880058288574</v>
       </c>
       <c r="D8" s="1">
-        <v>1.9185069799423218</v>
+        <v>1.968997597694397</v>
       </c>
     </row>
     <row r="9">
@@ -193,13 +193,13 @@
         <v>8</v>
       </c>
       <c r="B9" s="1">
-        <v>99.53228759765625</v>
+        <v>99.457733154296875</v>
       </c>
       <c r="C9" s="1">
-        <v>-0.167093425989151</v>
+        <v>-0.25193247199058533</v>
       </c>
       <c r="D9" s="1">
-        <v>0.67336726188659668</v>
+        <v>0.60457837581634521</v>
       </c>
     </row>
     <row r="10">
@@ -207,13 +207,13 @@
         <v>9</v>
       </c>
       <c r="B10" s="1">
-        <v>124.6224365234375</v>
+        <v>115.80441284179688</v>
       </c>
       <c r="C10" s="1">
-        <v>5.0539946556091309</v>
+        <v>4.3055582046508789</v>
       </c>
       <c r="D10" s="1">
-        <v>0.73573750257492065</v>
+        <v>0.5911906361579895</v>
       </c>
     </row>
     <row r="11">
@@ -221,13 +221,13 @@
         <v>10</v>
       </c>
       <c r="B11" s="1">
-        <v>149.14256286621094</v>
+        <v>122.04225921630859</v>
       </c>
       <c r="C11" s="1">
-        <v>5.5931320190429688</v>
+        <v>3.9517755508422852</v>
       </c>
       <c r="D11" s="1">
-        <v>0.28113716840744019</v>
+        <v>0.6602790355682373</v>
       </c>
     </row>
     <row r="12">
@@ -235,13 +235,13 @@
         <v>11</v>
       </c>
       <c r="B12" s="1">
-        <v>116.40653991699219</v>
+        <v>106.31224822998047</v>
       </c>
       <c r="C12" s="1">
-        <v>3.4467711448669434</v>
+        <v>2.2163121700286865</v>
       </c>
       <c r="D12" s="1">
-        <v>-0.45113068819046021</v>
+        <v>-0.094798311591148376</v>
       </c>
     </row>
   </sheetData>

</xml_diff>